<commit_message>
Added ques and choices input
</commit_message>
<xml_diff>
--- a/OMR/students.xlsx
+++ b/OMR/students.xlsx
@@ -412,7 +412,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A10"/>
+  <dimension ref="A1:A15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="M10" sqref="M10"/>
@@ -472,6 +472,31 @@
         <v>80</v>
       </c>
     </row>
+    <row r="11">
+      <c r="A11" t="n">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="n">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="n">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="n">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="n">
+        <v>70</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>